<commit_message>
Correct hourly gas shape
</commit_message>
<xml_diff>
--- a/data/residential_model/_EXCELFILES/lookup_dwelling_type.xlsx
+++ b/data/residential_model/_EXCELFILES/lookup_dwelling_type.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Detached</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>End-Terrace</t>
+  </si>
+  <si>
+    <t>TERRACED</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +516,22 @@
       </c>
       <c r="B7" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>